<commit_message>
After 11 week pass
</commit_message>
<xml_diff>
--- a/public/Sales_Report.xlsx
+++ b/public/Sales_Report.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Sales Report</t>
   </si>
   <si>
-    <t>From: 2025-01-19 To: 2025-01-30</t>
+    <t>From: 2025-03-03 To: 2025-03-04</t>
   </si>
   <si>
     <t>S.No</t>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>Payment Method</t>
+  </si>
+  <si>
+    <t>Anbu Kumar</t>
+  </si>
+  <si>
+    <t>2025-03-03</t>
+  </si>
+  <si>
+    <t>94.40</t>
+  </si>
+  <si>
+    <t>COD</t>
   </si>
   <si>
     <t>Total Order Amount:</t>
@@ -87,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -96,6 +108,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -442,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -503,44 +518,70 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="D5"/>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="6">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="7">
+        <v>320</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A4:B4"/>
@@ -549,10 +590,16 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="I7:L7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="I8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>